<commit_message>
update plan: use ADO.Net
</commit_message>
<xml_diff>
--- a/Plan/Project Plan.xlsx
+++ b/Plan/Project Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>Subjects</t>
   </si>
@@ -122,6 +122,19 @@
   </si>
   <si>
     <t>Tạo chương trình Winform như trong thư mục Exercises</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Kết nối cơ sở dữ liệu từ C#.Net sang sql sever</t>
+  </si>
+  <si>
+    <t>Làm quen với ADO.Net</t>
+  </si>
+  <si>
+    <t>sử dụng thư viện System.Data.sqlClient;
+Tài liệu hướng dẫn xem trong Document\CommandADO\Tao mot ket noi toi co so du lieu dung C#.pdf Từ trang 1-4</t>
   </si>
 </sst>
 </file>
@@ -131,7 +144,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1010409]d\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +157,15 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
@@ -170,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -193,6 +215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -654,9 +677,33 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="57" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="6">
+        <v>41335</v>
+      </c>
+      <c r="F6" s="6">
+        <v>41335</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -821,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -862,8 +909,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
@@ -880,5 +927,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
read and write file
</commit_message>
<xml_diff>
--- a/Plan/Project Plan.xlsx
+++ b/Plan/Project Plan.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>Subjects</t>
   </si>
@@ -213,6 +213,19 @@
   </si>
   <si>
     <t>21</t>
+  </si>
+  <si>
+    <t>_Tạo đối tượng StreamWriter strW = new StreamWriter(@"C:\test.txt");
+_Gọi hàm của đối tượng vừa tạo strW.Write(chuỗi cần ghi viết ở đây)
+_Nhớ khai báo thư viện System.IO</t>
+  </si>
+  <si>
+    <t>Tạo một form gồm 1 nút bấm button và một textbox. 
+Khi bấm vào button thì chữ ở ô text sẽ được lưu xuống file có tên là C:\test.txt chẳng hạn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_Làm quen với đối tượng ghi dữ liệu
+</t>
   </si>
 </sst>
 </file>
@@ -597,15 +610,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.625" style="5" customWidth="1"/>
     <col min="2" max="2" width="7.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45" customWidth="1"/>
+    <col min="3" max="3" width="50.875" customWidth="1"/>
     <col min="4" max="4" width="66.875" customWidth="1"/>
     <col min="5" max="7" width="15.625" style="6" customWidth="1"/>
     <col min="8" max="8" width="10.5" style="5" customWidth="1"/>
@@ -690,6 +703,9 @@
       <c r="F3" s="6">
         <v>41333</v>
       </c>
+      <c r="G3" s="6">
+        <v>41333</v>
+      </c>
       <c r="H3" s="5" t="s">
         <v>12</v>
       </c>
@@ -716,6 +732,9 @@
       <c r="F4" s="6">
         <v>41332</v>
       </c>
+      <c r="G4" s="6">
+        <v>41332</v>
+      </c>
       <c r="H4" s="5" t="s">
         <v>12</v>
       </c>
@@ -745,6 +764,9 @@
       <c r="F5" s="6">
         <v>41334</v>
       </c>
+      <c r="G5" s="6">
+        <v>41336</v>
+      </c>
       <c r="H5" s="5" t="s">
         <v>12</v>
       </c>
@@ -839,12 +861,33 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="6">
+        <v>41397</v>
+      </c>
+      <c r="F9" s="6">
+        <v>41338</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>